<commit_message>
Resultados e Algumas alterações
</commit_message>
<xml_diff>
--- a/resultadosV2.xlsx
+++ b/resultadosV2.xlsx
@@ -1,24 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lite\Documents\Github\MetroRealm\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="12795"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
     <sheet name="Planilha4" sheetId="4" r:id="rId4"/>
+    <sheet name="Plan1" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
   <si>
     <t>Itajaí - Navegantes</t>
   </si>
@@ -59,15 +54,51 @@
   <si>
     <t xml:space="preserve">   </t>
   </si>
+  <si>
+    <t>muito caro</t>
+  </si>
+  <si>
+    <t>levemente recomendado</t>
+  </si>
+  <si>
+    <t>não recomendado</t>
+  </si>
+  <si>
+    <t>não vale a pena</t>
+  </si>
+  <si>
+    <t>caro</t>
+  </si>
+  <si>
+    <t>barato</t>
+  </si>
+  <si>
+    <t>recomendado</t>
+  </si>
+  <si>
+    <t>muito barato</t>
+  </si>
+  <si>
+    <t>livre</t>
+  </si>
+  <si>
+    <t>levemente lento</t>
+  </si>
+  <si>
+    <t>lento</t>
+  </si>
+  <si>
+    <t>parado</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,16 +114,95 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3737"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCD2D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -100,20 +210,140 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6600"/>
+      <color rgb="FFFF3737"/>
+      <color rgb="FFFFCD2D"/>
+      <color rgb="FF292929"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -126,7 +356,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -165,6 +395,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -173,26 +404,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -260,7 +471,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-27D6-4A4B-B030-B5091192046F}"/>
             </c:ext>
@@ -325,7 +536,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-27D6-4A4B-B030-B5091192046F}"/>
             </c:ext>
@@ -340,11 +551,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="387410816"/>
-        <c:axId val="387410160"/>
+        <c:axId val="633740288"/>
+        <c:axId val="198052096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="387410816"/>
+        <c:axId val="633740288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -387,7 +598,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387410160"/>
+        <c:crossAx val="198052096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -395,7 +606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="387410160"/>
+        <c:axId val="198052096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -446,7 +657,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387410816"/>
+        <c:crossAx val="633740288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -460,6 +671,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -527,7 +739,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -566,6 +778,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -574,26 +787,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -655,7 +848,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6A82-44E4-83A3-26FD805D85ED}"/>
             </c:ext>
@@ -715,7 +908,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6A82-44E4-83A3-26FD805D85ED}"/>
             </c:ext>
@@ -775,7 +968,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6A82-44E4-83A3-26FD805D85ED}"/>
             </c:ext>
@@ -835,7 +1028,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-6A82-44E4-83A3-26FD805D85ED}"/>
             </c:ext>
@@ -849,12 +1042,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="390313896"/>
-        <c:axId val="390314224"/>
+        <c:axId val="633737216"/>
+        <c:axId val="198054400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="390313896"/>
+        <c:axId val="633737216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -896,7 +1090,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="390314224"/>
+        <c:crossAx val="198054400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -904,7 +1098,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="390314224"/>
+        <c:axId val="198054400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -955,7 +1149,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="390313896"/>
+        <c:crossAx val="633737216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -969,6 +1163,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1036,7 +1231,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -1080,6 +1275,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1088,26 +1284,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1196,7 +1372,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7570-46C8-A166-2A5EECA8B3D8}"/>
             </c:ext>
@@ -1283,7 +1459,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7570-46C8-A166-2A5EECA8B3D8}"/>
             </c:ext>
@@ -1370,7 +1546,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-7570-46C8-A166-2A5EECA8B3D8}"/>
             </c:ext>
@@ -1457,7 +1633,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-7570-46C8-A166-2A5EECA8B3D8}"/>
             </c:ext>
@@ -1471,12 +1647,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="455880584"/>
-        <c:axId val="455883536"/>
+        <c:axId val="635164672"/>
+        <c:axId val="198056704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="455880584"/>
+        <c:axId val="635164672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1519,7 +1696,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455883536"/>
+        <c:crossAx val="198056704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1527,7 +1704,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455883536"/>
+        <c:axId val="198056704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1578,7 +1755,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455880584"/>
+        <c:crossAx val="635164672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1592,6 +1769,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1659,7 +1837,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -1698,6 +1876,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1706,26 +1885,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1814,7 +1973,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-BAD4-42D9-AFAA-13773747E8E1}"/>
             </c:ext>
@@ -1901,7 +2060,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-BAD4-42D9-AFAA-13773747E8E1}"/>
             </c:ext>
@@ -1988,7 +2147,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-BAD4-42D9-AFAA-13773747E8E1}"/>
             </c:ext>
@@ -2075,7 +2234,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-BAD4-42D9-AFAA-13773747E8E1}"/>
             </c:ext>
@@ -2089,12 +2248,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="453744408"/>
-        <c:axId val="453739816"/>
+        <c:axId val="636010496"/>
+        <c:axId val="636183680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="453744408"/>
+        <c:axId val="636010496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2137,7 +2297,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453739816"/>
+        <c:crossAx val="636183680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2145,7 +2305,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="453739816"/>
+        <c:axId val="636183680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2196,7 +2356,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453744408"/>
+        <c:crossAx val="636010496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2210,6 +2370,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2277,7 +2438,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -2291,6 +2452,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2425,7 +2587,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F570-4E89-B976-68E34F063D27}"/>
             </c:ext>
@@ -2530,7 +2692,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F570-4E89-B976-68E34F063D27}"/>
             </c:ext>
@@ -2635,7 +2797,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-F570-4E89-B976-68E34F063D27}"/>
             </c:ext>
@@ -2740,7 +2902,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-F570-4E89-B976-68E34F063D27}"/>
             </c:ext>
@@ -2833,7 +2995,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-F570-4E89-B976-68E34F063D27}"/>
             </c:ext>
@@ -2926,7 +3088,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-F570-4E89-B976-68E34F063D27}"/>
             </c:ext>
@@ -3021,7 +3183,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-F570-4E89-B976-68E34F063D27}"/>
             </c:ext>
@@ -3035,12 +3197,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="313859000"/>
-        <c:axId val="311197920"/>
+        <c:axId val="636103168"/>
+        <c:axId val="636185984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="313859000"/>
+        <c:axId val="636103168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3083,7 +3246,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="311197920"/>
+        <c:crossAx val="636185984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3091,7 +3254,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="311197920"/>
+        <c:axId val="636185984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3142,7 +3305,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313859000"/>
+        <c:crossAx val="636103168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3156,6 +3319,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6750,7 +6914,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6760,7 +6924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -7426,4 +7590,173 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1.9</v>
+      </c>
+      <c r="C2" s="8">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1.3</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="E9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="E10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E13" s="11"/>
+      <c r="F13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>